<commit_message>
modified .gitignore to include excel files
</commit_message>
<xml_diff>
--- a/YAS_Performer/Data/Config.xlsx
+++ b/YAS_Performer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashen\Desktop\Revature\YoutubeAutomationSuite\YAS_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashen\Desktop\Revature\gavin-gilbert-code\week6\UiPath_REFWDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1DBBE5-B7AE-4BFA-B546-A6BA413888D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A549C-AFC2-4E9C-8FD8-7C4B3D483552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="2775" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -159,10 +159,7 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>YAS_Transactions</t>
-  </si>
-  <si>
-    <t>Shared</t>
+    <t>Product_Queue</t>
   </si>
 </sst>
 </file>
@@ -601,9 +598,7 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2787,7 +2782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>